<commit_message>
updated to M3 hardware
</commit_message>
<xml_diff>
--- a/MiniRhexHardware.xlsx
+++ b/MiniRhexHardware.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Monica/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\miniRHex\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80778D0A-2189-48D2-B5F6-5EED47434C52}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -59,9 +60,6 @@
     <t>Screws</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#92005a076/=1cvfwje</t>
-  </si>
-  <si>
     <t>Dynamixels</t>
   </si>
   <si>
@@ -89,9 +87,6 @@
     <t>Nuts</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#93625a102/=1cvfxju</t>
-  </si>
-  <si>
     <t>Bluetooth</t>
   </si>
   <si>
@@ -101,13 +96,19 @@
     <t>Spacer</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#93657a212/=1cvg4m2</t>
+    <t>https://www.mcmaster.com/#94500A223</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#90576A102</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#93657A203</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -172,6 +173,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -439,16 +443,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +469,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -482,7 +486,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -499,7 +503,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -516,7 +520,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -531,16 +535,16 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>4.25</v>
+        <v>6.08</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -548,16 +552,16 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>131.4</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -565,16 +569,16 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>23.79</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -582,16 +586,16 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>6.49</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -599,16 +603,16 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
         <v>5.73</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -616,16 +620,16 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2">
-        <v>9.84</v>
+        <v>3.36</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -633,16 +637,16 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>32.9</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -650,12 +654,12 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2">
-        <v>5.4</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
@@ -667,7 +671,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -680,17 +684,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4" location="92005a076/=1cvfwje"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8" location="acrylic/=1cvfzgg"/>
-    <hyperlink ref="D11" r:id="rId9" location="93625a102/=1cvfxju"/>
-    <hyperlink ref="D12" r:id="rId10"/>
-    <hyperlink ref="D13" r:id="rId11" location="93657a212/=1cvg4m2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D10" r:id="rId7" location="acrylic/=1cvfzgg" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated appearance and added quantity needed per robot
</commit_message>
<xml_diff>
--- a/MiniRhexHardware.xlsx
+++ b/MiniRhexHardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\miniRHex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80778D0A-2189-48D2-B5F6-5EED47434C52}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A801386A-BD35-4AA6-BC20-9E3BBF3B8B98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="16010" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Item</t>
   </si>
@@ -54,9 +54,6 @@
     <t>https://www.amazon.com/Performix-11602-6-075815116024-Yellow-Plasti/dp/B000ZN1T16/ref=sr_1_13?ie=UTF8&amp;qid=1526518098&amp;sr=8-13&amp;keywords=plastidip</t>
   </si>
   <si>
-    <t>3D printed parts</t>
-  </si>
-  <si>
     <t>Screws</t>
   </si>
   <si>
@@ -78,18 +75,12 @@
     <t>https://www.amazon.com/eBoot-Connector-Female-Cable-Battery/dp/B01M5AHF0Z</t>
   </si>
   <si>
-    <t>acrylic</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/#acrylic/=1cvfzgg</t>
   </si>
   <si>
     <t>Nuts</t>
   </si>
   <si>
-    <t>Bluetooth</t>
-  </si>
-  <si>
     <t>http://www.robotis.us/bt-210/</t>
   </si>
   <si>
@@ -103,25 +94,64 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/#93657A203</t>
+  </si>
+  <si>
+    <t>Amazon Parts</t>
+  </si>
+  <si>
+    <t>Robotis Parts</t>
+  </si>
+  <si>
+    <t>McMaster-Carr Parts</t>
+  </si>
+  <si>
+    <t>3D Printed Parts</t>
+  </si>
+  <si>
+    <t>Quantity per Robot</t>
+  </si>
+  <si>
+    <t>Servo Holder</t>
+  </si>
+  <si>
+    <t>Leg</t>
+  </si>
+  <si>
+    <t>Battery Holder</t>
+  </si>
+  <si>
+    <t>Short Servo Leg Hub</t>
+  </si>
+  <si>
+    <t>Long Servo Leg Hub</t>
+  </si>
+  <si>
+    <t>Total Printing</t>
+  </si>
+  <si>
+    <t>Bluetooth (optional)</t>
+  </si>
+  <si>
+    <t>https://github.com/robomechanics/MiniRHex/tree/master/CAD</t>
+  </si>
+  <si>
+    <t>1/8" acrylic, 7.5" x 4"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,6 +165,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,13 +206,41 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,255 +522,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.9140625" customWidth="1"/>
+    <col min="2" max="2" width="9.58203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11" style="9" customWidth="1"/>
+    <col min="4" max="4" width="201.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6">
+        <v>44</v>
+      </c>
+      <c r="C3" s="14">
+        <v>6.08</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6">
+        <v>32</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3.36</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
+        <v>5.73</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14">
+        <v>8.99</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14">
+        <v>9.52</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14">
+        <v>23.79</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14">
+        <v>6.49</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="14">
         <v>19.899999999999999</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="D13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>8.99</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>9.52</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="C14" s="14">
+        <v>131.4</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="14">
+        <v>32.9</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>6.08</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>131.4</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2">
-        <v>23.79</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2">
-        <v>6.49</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2">
-        <v>5.73</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6">
+        <v>6</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="6">
+        <v>4</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="6">
+        <v>6</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="14">
         <v>18</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2">
-        <v>3.36</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2">
-        <v>32.9</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A16:C16"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D10" r:id="rId7" location="acrylic/=1cvfzgg" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D5" r:id="rId7" location="acrylic/=1cvfzgg" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D3" r:id="rId9" location="94500A223" xr:uid="{69B4B288-1780-4489-9A12-854551DFE2C1}"/>
+    <hyperlink ref="D17" r:id="rId10" xr:uid="{7948E42C-FFE8-4717-B02F-F120771B861B}"/>
+    <hyperlink ref="D6" r:id="rId11" location="93657A203" xr:uid="{DE182A2C-07F2-4301-83AF-60BAF4E18B4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>